<commit_message>
updated code to remove redundant columns
</commit_message>
<xml_diff>
--- a/Support_mk/raw_data_column_description.xlsx
+++ b/Support_mk/raw_data_column_description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twin_\Desktop\UofT CES - Data Analytics Boot Camp\Class Work\module 20\capstone-project\Support_mk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6990C13-37C2-4544-ADD0-80E566A360A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6C57B9-6F75-4B91-A9AF-8CFD3B5DBE71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14020" yWindow="-16310" windowWidth="29020" windowHeight="15820" activeTab="1" xr2:uid="{A339BF75-A586-4EF9-94DC-E0C428B347E1}"/>
+    <workbookView xWindow="-11180" yWindow="-15860" windowWidth="25420" windowHeight="15370" xr2:uid="{A339BF75-A586-4EF9-94DC-E0C428B347E1}"/>
   </bookViews>
   <sheets>
     <sheet name="covid_stats_df" sheetId="3" r:id="rId1"/>
@@ -728,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F98E33-B317-4C72-88F0-1EBFF0433D7B}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -992,9 +992,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D623BF-3039-44C1-9C37-606D779ECE50}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P37" sqref="P37"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
updated cleaning of both dataframes
</commit_message>
<xml_diff>
--- a/Support_mk/raw_data_column_description.xlsx
+++ b/Support_mk/raw_data_column_description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twin_\Desktop\UofT CES - Data Analytics Boot Camp\Class Work\module 20\capstone-project\Support_mk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6C57B9-6F75-4B91-A9AF-8CFD3B5DBE71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF24BE5-818D-48E0-B333-644F6AC00A0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11180" yWindow="-15860" windowWidth="25420" windowHeight="15370" xr2:uid="{A339BF75-A586-4EF9-94DC-E0C428B347E1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A339BF75-A586-4EF9-94DC-E0C428B347E1}"/>
   </bookViews>
   <sheets>
     <sheet name="covid_stats_df" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="95">
   <si>
     <t>iso_code</t>
   </si>
@@ -728,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F98E33-B317-4C72-88F0-1EBFF0433D7B}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -908,78 +908,123 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="B27" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="B28" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="B29" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="B30" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="B31" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="A32" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="B32" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="B33" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="B34" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="B35" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="B36" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="B37" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="B38" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="B39" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="B40" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
         <v>38</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -992,9 +1037,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D623BF-3039-44C1-9C37-606D779ECE50}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>